<commit_message>
Updated file (4) 11.10.22
</commit_message>
<xml_diff>
--- a/LR3/table_1_109.xlsx
+++ b/LR3/table_1_109.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Никита\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B753DA2B-3C2C-457E-AF57-45423C60243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E323B9-B6A7-4958-8C20-F40A12FE9072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{0C8AD69E-E27F-4C5C-B274-39ABC1D21F9C}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{0C8AD69E-E27F-4C5C-B274-39ABC1D21F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AB1EC7-D742-455B-B481-2F223E49D7A6}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2064,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>IF(A34+1&lt;33,D$3,D$3*0.5)</f>
+        <f>D3/2</f>
         <v>59.95</v>
       </c>
       <c r="E35" s="1">
@@ -2109,7 +2109,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="10">IF(A35+1&lt;33,D$3,D$3*0.5)</f>
+        <f t="shared" ref="D36:D38" si="10">D4/2</f>
         <v>59.95</v>
       </c>
       <c r="E36" s="1">

</xml_diff>

<commit_message>
Updated file (5) 11.10.22
</commit_message>
<xml_diff>
--- a/LR3/table_1_109.xlsx
+++ b/LR3/table_1_109.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E323B9-B6A7-4958-8C20-F40A12FE9072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FB776D-033B-4489-978C-D4529E2DDD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{0C8AD69E-E27F-4C5C-B274-39ABC1D21F9C}"/>
+    <workbookView xWindow="4095" yWindow="1800" windowWidth="21600" windowHeight="11430" xr2:uid="{0C8AD69E-E27F-4C5C-B274-39ABC1D21F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -244,7 +244,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -260,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -300,7 +300,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -406,7 +406,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AB1EC7-D742-455B-B481-2F223E49D7A6}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -669,11 +669,11 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D34" si="0">$A$1*1.1</f>
+        <f>D3</f>
         <v>119.9</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E38" si="1">C4*D4</f>
+        <f t="shared" ref="E4:E38" si="0">C4*D4</f>
         <v>8333.0500000000011</v>
       </c>
       <c r="F4" s="3">
@@ -685,7 +685,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f>IF(G3+1&lt;F3+1, H3, H3+1)</f>
+        <f>IF(G3&gt;F3,G3-F3,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
@@ -693,17 +693,17 @@
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J38" si="2">H4*I4</f>
+        <f t="shared" ref="J4:J38" si="1">H4*I4</f>
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K38" si="3">E4+J4</f>
+        <f t="shared" ref="K4:K38" si="2">E4+J4</f>
         <v>8333.0500000000011</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A38" si="4">A4+1</f>
+        <f t="shared" ref="A5:A38" si="3">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -714,11 +714,11 @@
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D5:D34" si="4">D4</f>
         <v>119.9</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8273.1</v>
       </c>
       <c r="F5" s="3">
@@ -730,7 +730,7 @@
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H37" si="7">IF(G4+1&lt;F4+1, H4, H4+1)</f>
+        <f t="shared" ref="H5:H38" si="7">IF(G4&gt;F4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
@@ -738,17 +738,17 @@
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8273.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -759,11 +759,11 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8213.15</v>
       </c>
       <c r="F6" s="3">
@@ -783,17 +783,17 @@
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8213.15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -804,11 +804,11 @@
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8153.2000000000007</v>
       </c>
       <c r="F7" s="3">
@@ -828,17 +828,17 @@
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8153.2000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -849,11 +849,11 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8093.25</v>
       </c>
       <c r="F8" s="3">
@@ -873,17 +873,17 @@
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8093.25</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -894,11 +894,11 @@
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8033.3</v>
       </c>
       <c r="F9" s="3">
@@ -918,17 +918,17 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8033.3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -939,11 +939,11 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7973.35</v>
       </c>
       <c r="F10" s="3">
@@ -963,17 +963,17 @@
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7973.35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -984,11 +984,11 @@
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7913.4000000000005</v>
       </c>
       <c r="F11" s="3">
@@ -1008,17 +1008,17 @@
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7913.4000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1029,11 +1029,11 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7853.4500000000007</v>
       </c>
       <c r="F12" s="3">
@@ -1046,24 +1046,24 @@
       </c>
       <c r="H12" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="3"/>
-        <v>7863.4500000000007</v>
+        <f t="shared" si="2"/>
+        <v>7853.4500000000007</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1074,11 +1074,11 @@
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7793.5</v>
       </c>
       <c r="F13" s="3">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
-        <v>7813.5</v>
+        <f t="shared" si="2"/>
+        <v>7803.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1119,11 +1119,11 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7733.55</v>
       </c>
       <c r="F14" s="3">
@@ -1136,24 +1136,24 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="3"/>
-        <v>7763.55</v>
+        <f t="shared" si="2"/>
+        <v>7753.55</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1164,11 +1164,11 @@
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7673.6</v>
       </c>
       <c r="F15" s="3">
@@ -1181,24 +1181,24 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="3"/>
-        <v>7713.6</v>
+        <f t="shared" si="2"/>
+        <v>7703.6</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1209,11 +1209,11 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7613.6500000000005</v>
       </c>
       <c r="F16" s="3">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="3"/>
-        <v>7663.6500000000005</v>
+        <f t="shared" si="2"/>
+        <v>7653.6500000000005</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1254,11 +1254,11 @@
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7553.7000000000007</v>
       </c>
       <c r="F17" s="3">
@@ -1271,24 +1271,24 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="3"/>
-        <v>7613.7000000000007</v>
+        <f t="shared" si="2"/>
+        <v>7603.7000000000007</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1299,11 +1299,11 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7493.75</v>
       </c>
       <c r="F18" s="3">
@@ -1316,24 +1316,24 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="2"/>
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="3"/>
-        <v>7563.75</v>
+        <f t="shared" si="2"/>
+        <v>7553.75</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1344,11 +1344,11 @@
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7433.8</v>
       </c>
       <c r="F19" s="3">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="2"/>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="3"/>
-        <v>7513.8</v>
+        <f t="shared" si="2"/>
+        <v>7503.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1389,11 +1389,11 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7373.85</v>
       </c>
       <c r="F20" s="3">
@@ -1406,24 +1406,24 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="2"/>
-        <v>90</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="3"/>
-        <v>7463.85</v>
+        <f t="shared" si="2"/>
+        <v>7453.85</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1434,11 +1434,11 @@
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7313.9000000000005</v>
       </c>
       <c r="F21" s="3">
@@ -1451,24 +1451,24 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="3"/>
-        <v>7413.9000000000005</v>
+        <f t="shared" si="2"/>
+        <v>7403.9000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1479,11 +1479,11 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7253.9500000000007</v>
       </c>
       <c r="F22" s="3">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="2"/>
-        <v>110</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="3"/>
-        <v>7363.9500000000007</v>
+        <f t="shared" si="2"/>
+        <v>7353.9500000000007</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1524,11 +1524,11 @@
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7194</v>
       </c>
       <c r="F23" s="3">
@@ -1541,24 +1541,24 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="3"/>
-        <v>7314</v>
+        <f t="shared" si="2"/>
+        <v>7304</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1569,11 +1569,11 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7134.05</v>
       </c>
       <c r="F24" s="3">
@@ -1586,24 +1586,24 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="2"/>
-        <v>130</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="3"/>
-        <v>7264.05</v>
+        <f t="shared" si="2"/>
+        <v>7254.05</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1614,11 +1614,11 @@
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7074.1</v>
       </c>
       <c r="F25" s="3">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="H25" s="1">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="2"/>
-        <v>140</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="3"/>
-        <v>7214.1</v>
+        <f t="shared" si="2"/>
+        <v>7204.1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1659,11 +1659,11 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7014.1500000000005</v>
       </c>
       <c r="F26" s="3">
@@ -1676,24 +1676,24 @@
       </c>
       <c r="H26" s="1">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <f t="shared" si="1"/>
+        <v>140</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="3"/>
-        <v>7164.1500000000005</v>
+        <f t="shared" si="2"/>
+        <v>7154.1500000000005</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1704,11 +1704,11 @@
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6954.2000000000007</v>
       </c>
       <c r="F27" s="3">
@@ -1721,24 +1721,24 @@
       </c>
       <c r="H27" s="1">
         <f t="shared" si="7"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f t="shared" si="1"/>
+        <v>150</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="3"/>
-        <v>7114.2000000000007</v>
+        <f t="shared" si="2"/>
+        <v>7104.2000000000007</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1749,11 +1749,11 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6894.25</v>
       </c>
       <c r="F28" s="3">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="H28" s="1">
         <f t="shared" si="7"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="2"/>
-        <v>170</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="3"/>
-        <v>7064.25</v>
+        <f t="shared" si="2"/>
+        <v>7054.25</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1794,11 +1794,11 @@
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6834.3</v>
       </c>
       <c r="F29" s="3">
@@ -1811,24 +1811,24 @@
       </c>
       <c r="H29" s="1">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="2"/>
-        <v>180</v>
+        <f t="shared" si="1"/>
+        <v>170</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="3"/>
-        <v>7014.3</v>
+        <f t="shared" si="2"/>
+        <v>7004.3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1839,11 +1839,11 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6774.35</v>
       </c>
       <c r="F30" s="3">
@@ -1856,24 +1856,24 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" si="7"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="2"/>
-        <v>190</v>
+        <f t="shared" si="1"/>
+        <v>180</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="3"/>
-        <v>6964.35</v>
+        <f t="shared" si="2"/>
+        <v>6954.35</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1884,11 +1884,11 @@
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6714.4000000000005</v>
       </c>
       <c r="F31" s="3">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="H31" s="1">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="2"/>
-        <v>200</v>
+        <f t="shared" si="1"/>
+        <v>190</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="3"/>
-        <v>6914.4000000000005</v>
+        <f t="shared" si="2"/>
+        <v>6904.4000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1929,11 +1929,11 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6654.4500000000007</v>
       </c>
       <c r="F32" s="3">
@@ -1946,24 +1946,24 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" si="7"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="2"/>
-        <v>210</v>
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="3"/>
-        <v>6864.4500000000007</v>
+        <f t="shared" si="2"/>
+        <v>6854.4500000000007</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1974,11 +1974,11 @@
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6594.5</v>
       </c>
       <c r="F33" s="3">
@@ -1991,24 +1991,24 @@
       </c>
       <c r="H33" s="1">
         <f t="shared" si="7"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="2"/>
-        <v>220</v>
+        <f t="shared" si="1"/>
+        <v>210</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="3"/>
-        <v>6814.5</v>
+        <f t="shared" si="2"/>
+        <v>6804.5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2019,11 +2019,11 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119.9</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6534.55</v>
       </c>
       <c r="F34" s="3">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" si="7"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="2"/>
-        <v>230</v>
+        <f t="shared" si="1"/>
+        <v>220</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="3"/>
-        <v>6764.55</v>
+        <f t="shared" si="2"/>
+        <v>6754.55</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2068,7 +2068,7 @@
         <v>59.95</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3237.3</v>
       </c>
       <c r="F35" s="3">
@@ -2081,24 +2081,24 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" si="7"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="1"/>
+        <v>230</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="3"/>
-        <v>3477.3</v>
+        <f t="shared" si="2"/>
+        <v>3467.3</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2113,7 +2113,7 @@
         <v>59.95</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3207.3250000000003</v>
       </c>
       <c r="F36" s="3">
@@ -2126,24 +2126,24 @@
       </c>
       <c r="H36" s="1">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="2"/>
-        <v>250</v>
+        <f t="shared" si="1"/>
+        <v>240</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="3"/>
-        <v>3457.3250000000003</v>
+        <f t="shared" si="2"/>
+        <v>3447.3250000000003</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2158,7 +2158,7 @@
         <v>59.95</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3177.3500000000004</v>
       </c>
       <c r="F37" s="3">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="H37" s="1">
         <f t="shared" si="7"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="2"/>
-        <v>260</v>
+        <f t="shared" si="1"/>
+        <v>250</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="3"/>
-        <v>3437.3500000000004</v>
+        <f t="shared" si="2"/>
+        <v>3427.3500000000004</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2203,7 +2203,7 @@
         <v>59.95</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3147.375</v>
       </c>
       <c r="F38" s="3">
@@ -2215,20 +2215,20 @@
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f>IF(G37+1&lt;F37+1, H37, H37+1)</f>
-        <v>27</v>
+        <f t="shared" si="7"/>
+        <v>26</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="2"/>
-        <v>270</v>
+        <f t="shared" si="1"/>
+        <v>260</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="3"/>
-        <v>3417.375</v>
+        <f t="shared" si="2"/>
+        <v>3407.375</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2236,8 +2236,8 @@
         <v>44</v>
       </c>
       <c r="C40" s="4">
-        <f>TRUNC(SUM(K3:K38))</f>
-        <v>255390</v>
+        <f>FLOOR(SUM(K3:K38),1)</f>
+        <v>255120</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="C42" s="4">
         <f>MAX(H3:H38)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated file (6) 11.10.22
</commit_message>
<xml_diff>
--- a/LR3/table_1_109.xlsx
+++ b/LR3/table_1_109.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FB776D-033B-4489-978C-D4529E2DDD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8791AE86-ECA6-4B4F-89DF-C3E29D068285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1800" windowWidth="21600" windowHeight="11430" xr2:uid="{0C8AD69E-E27F-4C5C-B274-39ABC1D21F9C}"/>
   </bookViews>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AB1EC7-D742-455B-B481-2F223E49D7A6}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -642,6 +642,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="1">
+        <f>IF(G3&gt;F3,G3-F3,0)</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -685,7 +686,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f>IF(G3&gt;F3,G3-F3,0)</f>
+        <f t="shared" ref="H4:H38" si="1">IF(G4&gt;F4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
@@ -693,17 +694,17 @@
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J38" si="1">H4*I4</f>
+        <f t="shared" ref="J4:J38" si="2">H4*I4</f>
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K38" si="2">E4+J4</f>
+        <f t="shared" ref="K4:K38" si="3">E4+J4</f>
         <v>8333.0500000000011</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A38" si="3">A4+1</f>
+        <f t="shared" ref="A5:A38" si="4">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -714,7 +715,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D34" si="4">D4</f>
+        <f t="shared" ref="D5:D34" si="5">D4</f>
         <v>119.9</v>
       </c>
       <c r="E5" s="1">
@@ -722,15 +723,15 @@
         <v>8273.1</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F38" si="5">F4</f>
+        <f t="shared" ref="F5:F38" si="6">F4</f>
         <v>44813</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G38" si="6">G4+1</f>
+        <f t="shared" ref="G5:G38" si="7">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H38" si="7">IF(G4&gt;F4,G4-F4,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
@@ -738,17 +739,17 @@
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8273.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -759,7 +760,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E6" s="1">
@@ -767,15 +768,15 @@
         <v>8213.15</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44808</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
@@ -783,17 +784,17 @@
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8213.15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -804,7 +805,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E7" s="1">
@@ -812,15 +813,15 @@
         <v>8153.2000000000007</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44809</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
@@ -828,17 +829,17 @@
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8153.2000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -849,7 +850,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E8" s="1">
@@ -857,15 +858,15 @@
         <v>8093.25</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44810</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
@@ -873,17 +874,17 @@
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8093.25</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -894,7 +895,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E9" s="1">
@@ -902,15 +903,15 @@
         <v>8033.3</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44811</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -918,17 +919,17 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8033.3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -939,7 +940,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E10" s="1">
@@ -947,15 +948,15 @@
         <v>7973.35</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44812</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
@@ -963,17 +964,17 @@
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7973.35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -984,7 +985,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E11" s="1">
@@ -992,15 +993,15 @@
         <v>7913.4000000000005</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I11" s="1">
@@ -1008,17 +1009,17 @@
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7913.4000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1029,7 +1030,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E12" s="1">
@@ -1037,33 +1038,33 @@
         <v>7853.4500000000007</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44814</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="2"/>
-        <v>7853.4500000000007</v>
+        <f t="shared" si="3"/>
+        <v>7863.4500000000007</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1074,7 +1075,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E13" s="1">
@@ -1082,33 +1083,33 @@
         <v>7793.5</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44815</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
-        <v>7803.5</v>
+        <f t="shared" si="3"/>
+        <v>7813.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1119,7 +1120,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E14" s="1">
@@ -1127,33 +1128,33 @@
         <v>7733.55</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="2"/>
-        <v>7753.55</v>
+        <f t="shared" si="3"/>
+        <v>7763.55</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1164,7 +1165,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E15" s="1">
@@ -1172,33 +1173,33 @@
         <v>7673.6</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44817</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="7"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="2"/>
-        <v>7703.6</v>
+        <f t="shared" si="3"/>
+        <v>7713.6</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1209,7 +1210,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E16" s="1">
@@ -1217,33 +1218,33 @@
         <v>7613.6500000000005</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44818</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="7"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="2"/>
+        <v>50</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="2"/>
-        <v>7653.6500000000005</v>
+        <f t="shared" si="3"/>
+        <v>7663.6500000000005</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1254,7 +1255,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E17" s="1">
@@ -1262,33 +1263,33 @@
         <v>7553.7000000000007</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44819</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="2"/>
+        <v>60</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="2"/>
-        <v>7603.7000000000007</v>
+        <f t="shared" si="3"/>
+        <v>7613.7000000000007</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1299,7 +1300,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E18" s="1">
@@ -1307,33 +1308,33 @@
         <v>7493.75</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44820</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" si="2"/>
+        <v>70</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="2"/>
-        <v>7553.75</v>
+        <f t="shared" si="3"/>
+        <v>7563.75</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1344,7 +1345,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E19" s="1">
@@ -1352,33 +1353,33 @@
         <v>7433.8</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44821</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f t="shared" si="2"/>
+        <v>80</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="2"/>
-        <v>7503.8</v>
+        <f t="shared" si="3"/>
+        <v>7513.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1389,7 +1390,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E20" s="1">
@@ -1397,33 +1398,33 @@
         <v>7373.85</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44822</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="7"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>90</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="2"/>
-        <v>7453.85</v>
+        <f t="shared" si="3"/>
+        <v>7463.85</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1434,7 +1435,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E21" s="1">
@@ -1442,33 +1443,33 @@
         <v>7313.9000000000005</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44823</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="7"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="2"/>
-        <v>7403.9000000000005</v>
+        <f t="shared" si="3"/>
+        <v>7413.9000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1479,7 +1480,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E22" s="1">
@@ -1487,33 +1488,33 @@
         <v>7253.9500000000007</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44824</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="2"/>
-        <v>7353.9500000000007</v>
+        <f t="shared" si="3"/>
+        <v>7363.9500000000007</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1524,7 +1525,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E23" s="1">
@@ -1532,33 +1533,33 @@
         <v>7194</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44825</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="7"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="1"/>
-        <v>110</v>
+        <f t="shared" si="2"/>
+        <v>120</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="2"/>
-        <v>7304</v>
+        <f t="shared" si="3"/>
+        <v>7314</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1569,7 +1570,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E24" s="1">
@@ -1577,33 +1578,33 @@
         <v>7134.05</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44826</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="7"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f t="shared" si="2"/>
+        <v>130</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="2"/>
-        <v>7254.05</v>
+        <f t="shared" si="3"/>
+        <v>7264.05</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1614,7 +1615,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E25" s="1">
@@ -1622,33 +1623,33 @@
         <v>7074.1</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44827</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="7"/>
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="1"/>
-        <v>130</v>
+        <f t="shared" si="2"/>
+        <v>140</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="2"/>
-        <v>7204.1</v>
+        <f t="shared" si="3"/>
+        <v>7214.1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1659,7 +1660,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E26" s="1">
@@ -1667,33 +1668,33 @@
         <v>7014.1500000000005</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44828</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="7"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="1"/>
-        <v>140</v>
+        <f t="shared" si="2"/>
+        <v>150</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="2"/>
-        <v>7154.1500000000005</v>
+        <f t="shared" si="3"/>
+        <v>7164.1500000000005</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1704,7 +1705,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E27" s="1">
@@ -1712,33 +1713,33 @@
         <v>6954.2000000000007</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44829</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="7"/>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="2"/>
+        <v>160</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="2"/>
-        <v>7104.2000000000007</v>
+        <f t="shared" si="3"/>
+        <v>7114.2000000000007</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1749,7 +1750,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E28" s="1">
@@ -1757,33 +1758,33 @@
         <v>6894.25</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44830</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <f t="shared" si="2"/>
+        <v>170</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="2"/>
-        <v>7054.25</v>
+        <f t="shared" si="3"/>
+        <v>7064.25</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1794,7 +1795,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E29" s="1">
@@ -1802,33 +1803,33 @@
         <v>6834.3</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44831</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="7"/>
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="1"/>
-        <v>170</v>
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="2"/>
-        <v>7004.3</v>
+        <f t="shared" si="3"/>
+        <v>7014.3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1839,7 +1840,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E30" s="1">
@@ -1847,33 +1848,33 @@
         <v>6774.35</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44832</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f t="shared" si="2"/>
+        <v>190</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="2"/>
-        <v>6954.35</v>
+        <f t="shared" si="3"/>
+        <v>6964.35</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1884,7 +1885,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E31" s="1">
@@ -1892,33 +1893,33 @@
         <v>6714.4000000000005</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44833</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="7"/>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="1"/>
-        <v>190</v>
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="2"/>
-        <v>6904.4000000000005</v>
+        <f t="shared" si="3"/>
+        <v>6914.4000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1929,7 +1930,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E32" s="1">
@@ -1937,33 +1938,33 @@
         <v>6654.4500000000007</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44834</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <f t="shared" si="2"/>
+        <v>210</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="2"/>
-        <v>6854.4500000000007</v>
+        <f t="shared" si="3"/>
+        <v>6864.4500000000007</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1974,7 +1975,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E33" s="1">
@@ -1982,33 +1983,33 @@
         <v>6594.5</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44835</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="7"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <f t="shared" si="2"/>
+        <v>220</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="2"/>
-        <v>6804.5</v>
+        <f t="shared" si="3"/>
+        <v>6814.5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2019,7 +2020,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.9</v>
       </c>
       <c r="E34" s="1">
@@ -2027,33 +2028,33 @@
         <v>6534.55</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44836</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="7"/>
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="1"/>
-        <v>220</v>
+        <f t="shared" si="2"/>
+        <v>230</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="2"/>
-        <v>6754.55</v>
+        <f t="shared" si="3"/>
+        <v>6764.55</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2072,33 +2073,33 @@
         <v>3237.3</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44837</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="7"/>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="1"/>
-        <v>230</v>
+        <f t="shared" si="2"/>
+        <v>240</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="2"/>
-        <v>3467.3</v>
+        <f t="shared" si="3"/>
+        <v>3477.3</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2109,7 +2110,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="10">D4/2</f>
+        <f>D3/2</f>
         <v>59.95</v>
       </c>
       <c r="E36" s="1">
@@ -2117,33 +2118,33 @@
         <v>3207.3250000000003</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44838</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="7"/>
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="1"/>
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>250</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="2"/>
-        <v>3447.3250000000003</v>
+        <f t="shared" si="3"/>
+        <v>3457.3250000000003</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2154,7 +2155,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="10"/>
+        <f>D3/2</f>
         <v>59.95</v>
       </c>
       <c r="E37" s="1">
@@ -2162,33 +2163,33 @@
         <v>3177.3500000000004</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44839</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="7"/>
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="1"/>
-        <v>250</v>
+        <f t="shared" si="2"/>
+        <v>260</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="2"/>
-        <v>3427.3500000000004</v>
+        <f t="shared" si="3"/>
+        <v>3437.3500000000004</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2199,7 +2200,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="10"/>
+        <f>D3/2</f>
         <v>59.95</v>
       </c>
       <c r="E38" s="1">
@@ -2207,28 +2208,28 @@
         <v>3147.375</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="7"/>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="1"/>
-        <v>260</v>
+        <f t="shared" si="2"/>
+        <v>270</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="2"/>
-        <v>3407.375</v>
+        <f t="shared" si="3"/>
+        <v>3417.375</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2237,7 +2238,7 @@
       </c>
       <c r="C40" s="4">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>255120</v>
+        <v>255390</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,7 +2256,7 @@
       </c>
       <c r="C42" s="4">
         <f>MAX(H3:H38)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>